<commit_message>
Actualizar WEEK, TASK, ultimas semanas
Actualizacion de scripts WEEK, TASK del equipo de las ultimas semanas
</commit_message>
<xml_diff>
--- a/NoteBook/task and schedule plans and actual/TASK_Layne.xlsx
+++ b/NoteBook/task and schedule plans and actual/TASK_Layne.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FabiánEduardo\Documents\GitHub\tsp\NoteBook\task and schedule plans and actual\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15555"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="TOTAL_HORAS">Hoja1!$D$38</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -609,18 +614,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,33 +667,6 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -712,6 +717,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1006,227 +1014,227 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="7.5" style="1" customWidth="1"/>
-    <col min="9" max="10" width="8.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="7.42578125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="8.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" style="16" customWidth="1"/>
     <col min="12" max="12" width="8" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" style="16" customWidth="1"/>
-    <col min="14" max="15" width="11.5" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="7.42578125" style="16" customWidth="1"/>
+    <col min="14" max="15" width="11.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="16" thickBot="1">
+    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="49">
         <v>41719</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-    </row>
-    <row r="4" spans="1:15" ht="16" thickBot="1">
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-    </row>
-    <row r="5" spans="1:15" ht="16" thickBot="1">
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+    </row>
+    <row r="5" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="32">
-        <v>1</v>
-      </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="1:15" ht="15" thickBot="1">
+      <c r="E5" s="44">
+        <v>1</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="16" thickBot="1">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="43" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="43" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="43" t="s">
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="44"/>
-      <c r="M7" s="45"/>
-    </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1">
-      <c r="A8" s="33" t="s">
+      <c r="L7" s="36"/>
+      <c r="M7" s="37"/>
+    </row>
+    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="47" t="s">
+      <c r="F8" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-    </row>
-    <row r="13" spans="1:15" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+    </row>
+    <row r="13" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
       <c r="N13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1234,8 +1242,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15" thickBot="1">
-      <c r="A14" s="41" t="s">
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="34" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="4"/>
@@ -1283,8 +1291,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1">
-      <c r="A15" s="35"/>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5" t="s">
         <v>24</v>
@@ -1330,8 +1338,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A16" s="42"/>
+    <row r="16" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5" t="s">
         <v>25</v>
@@ -1377,8 +1385,8 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6"/>
@@ -1427,8 +1435,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" thickBot="1">
-      <c r="A18" s="35"/>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5" t="s">
         <v>27</v>
@@ -1475,8 +1483,8 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1">
-      <c r="A19" s="35" t="s">
+    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="6"/>
@@ -1525,8 +1533,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="29" thickBot="1">
-      <c r="A20" s="35"/>
+    <row r="20" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
         <v>51</v>
@@ -1573,8 +1581,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" thickBot="1">
-      <c r="A21" s="35"/>
+    <row r="21" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5" t="s">
         <v>29</v>
@@ -1621,8 +1629,8 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" thickBot="1">
-      <c r="A22" s="35"/>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5" t="s">
         <v>45</v>
@@ -1669,8 +1677,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" thickBot="1">
-      <c r="A23" s="35"/>
+    <row r="23" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5" t="s">
         <v>30</v>
@@ -1717,8 +1725,8 @@
         <v>2.1999999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15" thickBot="1">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="32"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
         <v>31</v>
@@ -1765,8 +1773,8 @@
         <v>2.8000000000000007</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15" thickBot="1">
-      <c r="A25" s="42"/>
+    <row r="25" spans="1:15" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="33"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5" t="s">
         <v>32</v>
@@ -1813,8 +1821,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" thickBot="1">
-      <c r="A26" s="35"/>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="32"/>
       <c r="B26" s="6"/>
       <c r="C26" s="31" t="s">
         <v>52</v>
@@ -1858,8 +1866,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" thickBot="1">
-      <c r="A27" s="35"/>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="32"/>
       <c r="B27" s="6"/>
       <c r="C27" s="31" t="s">
         <v>53</v>
@@ -1902,8 +1910,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" thickBot="1">
-      <c r="A28" s="41" t="s">
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="34" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="6"/>
@@ -1948,8 +1956,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" thickBot="1">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="32"/>
       <c r="B29" s="6"/>
       <c r="C29" s="31" t="s">
         <v>33</v>
@@ -1992,8 +2000,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" thickBot="1">
-      <c r="A30" s="35" t="s">
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="6"/>
@@ -2025,11 +2033,11 @@
         <v>62</v>
       </c>
       <c r="K30" s="23">
-        <v>8.9</v>
+        <v>4</v>
       </c>
       <c r="L30" s="24">
         <f>K30+L29</f>
-        <v>28.147073216638432</v>
+        <v>23.247073216638434</v>
       </c>
       <c r="M30" s="23">
         <v>5</v>
@@ -2038,8 +2046,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" thickBot="1">
-      <c r="A31" s="35"/>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="32"/>
       <c r="B31" s="6"/>
       <c r="C31" s="21" t="s">
         <v>34</v>
@@ -2069,11 +2077,11 @@
         <v>78.599999999999994</v>
       </c>
       <c r="K31" s="23">
-        <v>18.3</v>
+        <v>8</v>
       </c>
       <c r="L31" s="24">
         <f>L30+K31</f>
-        <v>46.447073216638429</v>
+        <v>31.247073216638434</v>
       </c>
       <c r="M31" s="23">
         <v>5</v>
@@ -2082,8 +2090,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" thickBot="1">
-      <c r="A32" s="35"/>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="32"/>
       <c r="B32" s="6"/>
       <c r="C32" s="21" t="s">
         <v>46</v>
@@ -2115,7 +2123,7 @@
       </c>
       <c r="L32" s="24">
         <f t="shared" ref="L32:L37" si="5">K32+L31</f>
-        <v>49.347073216638428</v>
+        <v>34.147073216638432</v>
       </c>
       <c r="M32" s="23">
         <v>5</v>
@@ -2124,8 +2132,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" thickBot="1">
-      <c r="A33" s="35" t="s">
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B33" s="6"/>
@@ -2159,7 +2167,7 @@
       </c>
       <c r="L33" s="28">
         <f t="shared" si="5"/>
-        <v>51.047073216638431</v>
+        <v>35.847073216638435</v>
       </c>
       <c r="M33" s="27">
         <v>6</v>
@@ -2168,8 +2176,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" thickBot="1">
-      <c r="A34" s="35"/>
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="32"/>
       <c r="B34" s="6"/>
       <c r="C34" s="25" t="s">
         <v>47</v>
@@ -2201,7 +2209,7 @@
       </c>
       <c r="L34" s="28">
         <f t="shared" si="5"/>
-        <v>52.247073216638434</v>
+        <v>37.047073216638438</v>
       </c>
       <c r="M34" s="27">
         <v>6</v>
@@ -2210,8 +2218,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" thickBot="1">
-      <c r="A35" s="35"/>
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="32"/>
       <c r="B35" s="6"/>
       <c r="C35" s="25" t="s">
         <v>48</v>
@@ -2245,7 +2253,7 @@
       </c>
       <c r="L35" s="28">
         <f t="shared" si="5"/>
-        <v>53.247073216638434</v>
+        <v>38.047073216638438</v>
       </c>
       <c r="M35" s="27">
         <v>6</v>
@@ -2254,8 +2262,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" thickBot="1">
-      <c r="A36" s="35" t="s">
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="32" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="6"/>
@@ -2289,7 +2297,7 @@
       </c>
       <c r="L36" s="28">
         <f t="shared" si="5"/>
-        <v>56.047073216638431</v>
+        <v>40.847073216638435</v>
       </c>
       <c r="M36" s="27">
         <v>6</v>
@@ -2298,8 +2306,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" thickBot="1">
-      <c r="A37" s="42"/>
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="33"/>
       <c r="B37" s="6"/>
       <c r="C37" s="29" t="s">
         <v>37</v>
@@ -2333,7 +2341,7 @@
       </c>
       <c r="L37" s="28">
         <f t="shared" si="5"/>
-        <v>59.447073216638429</v>
+        <v>44.247073216638434</v>
       </c>
       <c r="M37" s="27">
         <v>6</v>
@@ -2342,7 +2350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15" thickBot="1">
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -2365,22 +2373,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="G8:G13"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E8:E13"/>
@@ -2397,6 +2389,22 @@
     <mergeCell ref="I8:I13"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2415,7 +2423,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2432,7 +2440,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>